<commit_message>
ajuste de pago semana 13
</commit_message>
<xml_diff>
--- a/Quiniela Semana 13 NFL 2025.xlsx
+++ b/Quiniela Semana 13 NFL 2025.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://citlali-my.sharepoint.com/personal/gaas_citlali_mx/Documents/Personal/Proyectos_personales/NFL/2025/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_F189B8770A6B7E1D046108DE8532AB21413A974F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8A49188-64E0-42FC-BABE-669027C1BDCF}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="13" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -196,8 +215,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,13 +224,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -223,24 +266,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -278,7 +339,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -312,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -346,9 +408,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -521,15 +584,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -584,8 +669,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -640,7 +725,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -696,8 +781,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -752,8 +837,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -808,8 +893,8 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
-      <c r="A6" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -864,8 +949,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -920,8 +1005,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
-      <c r="A8" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -976,8 +1061,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
-      <c r="A9" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1032,8 +1117,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
-      <c r="A10" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1088,8 +1173,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
-      <c r="A11" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1144,7 +1229,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1200,8 +1285,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
-      <c r="A13" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1256,8 +1341,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
-      <c r="A14" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1312,8 +1397,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
-      <c r="A15" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -1368,8 +1453,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
-      <c r="A16" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -1424,8 +1509,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
-      <c r="A17" t="s">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1480,8 +1565,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
-      <c r="A18" t="s">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1536,7 +1621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1592,7 +1677,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1648,8 +1733,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
-      <c r="A21" t="s">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1704,8 +1789,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
-      <c r="A22" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -1760,8 +1845,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
-      <c r="A23" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -1816,8 +1901,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
-      <c r="A24" t="s">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1872,8 +1957,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
-      <c r="A25" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -1928,7 +2013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1984,8 +2069,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
-      <c r="A27" t="s">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -2040,8 +2125,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
-      <c r="A28" t="s">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -2096,8 +2181,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
-      <c r="A29" t="s">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">

</xml_diff>